<commit_message>
Mult instr + B tests (missing neg imm)
</commit_message>
<xml_diff>
--- a/Instruction List.xlsx
+++ b/Instruction List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="142">
   <si>
     <t>ADD</t>
   </si>
@@ -444,6 +444,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Check for all branches negative condition</t>
+  </si>
+  <si>
+    <t>signextend(imm&lt;&lt;2) is bad</t>
   </si>
 </sst>
 </file>
@@ -599,21 +605,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -893,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:O61"/>
+  <dimension ref="C2:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -910,9 +916,10 @@
     <col min="10" max="10" width="11.1796875" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="0.1796875" customWidth="1"/>
     <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="13" max="13" width="27.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C2" s="9" t="s">
         <v>112</v>
       </c>
@@ -944,7 +951,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -988,7 +995,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C4" s="2" t="s">
         <v>104</v>
       </c>
@@ -1032,7 +1039,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1076,7 +1083,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="1" t="s">
         <v>74</v>
       </c>
@@ -1119,8 +1126,9 @@
       <c r="N6" s="8" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="7" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C7" s="2" t="s">
         <v>108</v>
       </c>
@@ -1164,7 +1172,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="2" t="s">
         <v>93</v>
       </c>
@@ -1208,7 +1216,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1252,7 +1260,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="3:14" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:16" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1296,7 +1304,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1340,7 +1348,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="2" t="s">
         <v>76</v>
       </c>
@@ -1384,7 +1392,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="1" t="s">
         <v>110</v>
       </c>
@@ -1428,7 +1436,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1472,7 +1480,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="2" t="s">
         <v>55</v>
       </c>
@@ -1516,7 +1524,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="1" t="s">
         <v>106</v>
       </c>
@@ -1733,7 +1741,7 @@
         <v>139</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1777,7 +1785,7 @@
         <v>139</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1909,7 +1917,7 @@
         <v>139</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1949,11 +1957,11 @@
 step_err =  SLLV (state, rs, rt, rd, sa);
 break;</v>
       </c>
-      <c r="L25" s="11" t="s">
+      <c r="L25" s="10" t="s">
         <v>139</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1999,7 +2007,7 @@
         <v>139</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="3:14" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2044,8 +2052,11 @@
       <c r="L27" s="8" t="s">
         <v>139</v>
       </c>
+      <c r="M27" t="s">
+        <v>140</v>
+      </c>
       <c r="N27" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2088,6 +2099,9 @@
       <c r="L28" s="8" t="s">
         <v>139</v>
       </c>
+      <c r="M28" t="s">
+        <v>141</v>
+      </c>
       <c r="N28" s="8" t="s">
         <v>136</v>
       </c>
@@ -2265,7 +2279,7 @@
         <v>139</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2309,7 +2323,7 @@
         <v>139</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="3:14" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2353,7 +2367,7 @@
         <v>139</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="3:14" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2397,7 +2411,7 @@
         <v>139</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2746,7 +2760,7 @@
 break;</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N43" s="8" t="s">
         <v>136</v>
@@ -2790,7 +2804,7 @@
 break;</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N44" s="8" t="s">
         <v>136</v>
@@ -2834,7 +2848,7 @@
 break;</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N45" s="8" t="s">
         <v>136</v>
@@ -2878,7 +2892,7 @@
 break;</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N46" s="8" t="s">
         <v>136</v>
@@ -2922,7 +2936,7 @@
 break;</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N47" s="8" t="s">
         <v>136</v>
@@ -2966,7 +2980,7 @@
 break;</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N48" s="8" t="s">
         <v>136</v>
@@ -3015,7 +3029,7 @@
         <v>139</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="3:15" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3061,7 +3075,7 @@
         <v>139</v>
       </c>
       <c r="N50" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="O50" s="12"/>
     </row>
@@ -3103,7 +3117,7 @@
 break;</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N51" s="8" t="s">
         <v>136</v>
@@ -3147,7 +3161,7 @@
 break;</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N52" s="8" t="s">
         <v>136</v>
@@ -3190,8 +3204,8 @@
 step_err =  DIV (state, rs, rt, rd, sa);
 break;</v>
       </c>
-      <c r="L53" s="8" t="s">
-        <v>136</v>
+      <c r="L53" s="10" t="s">
+        <v>139</v>
       </c>
       <c r="N53" s="8" t="s">
         <v>136</v>
@@ -3287,6 +3301,9 @@
     </row>
     <row r="56" spans="3:15" x14ac:dyDescent="0.35">
       <c r="I56" s="3"/>
+    </row>
+    <row r="59" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="N59" s="12"/>
     </row>
     <row r="61" spans="3:15" x14ac:dyDescent="0.35">
       <c r="H61" t="str">
@@ -3304,11 +3321,11 @@
     <sortCondition ref="I3:I55"/>
   </sortState>
   <conditionalFormatting sqref="L3:L55">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",L3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",L3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",L3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">

</xml_diff>

<commit_message>
LWL, LWR, mfthilo instr tests
</commit_message>
<xml_diff>
--- a/Instruction List.xlsx
+++ b/Instruction List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="140">
   <si>
     <t>ADD</t>
   </si>
@@ -444,12 +444,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Check for all branches negative condition</t>
-  </si>
-  <si>
-    <t>signextend(imm&lt;&lt;2) is bad</t>
   </si>
 </sst>
 </file>
@@ -901,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2052,9 +2046,6 @@
       <c r="L27" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="M27" t="s">
-        <v>140</v>
-      </c>
       <c r="N27" s="8" t="s">
         <v>139</v>
       </c>
@@ -2099,11 +2090,9 @@
       <c r="L28" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="M28" t="s">
-        <v>141</v>
-      </c>
+      <c r="M28" s="12"/>
       <c r="N28" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2235,7 +2224,7 @@
         <v>139</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="3:14" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2763,7 +2752,7 @@
         <v>139</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2807,7 +2796,7 @@
         <v>139</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2851,7 +2840,7 @@
         <v>139</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2895,7 +2884,7 @@
         <v>139</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3249,7 +3238,7 @@
 break;</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N54" s="8" t="s">
         <v>136</v>
@@ -3293,7 +3282,7 @@
 break;</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="N55" s="8" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
fixed load/store some instr + new jump tests
</commit_message>
<xml_diff>
--- a/Instruction List.xlsx
+++ b/Instruction List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="143">
   <si>
     <t>ADD</t>
   </si>
@@ -444,6 +444,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>YEs</t>
+  </si>
+  <si>
+    <t>Missing +/- and div by 0</t>
+  </si>
+  <si>
+    <t>missing div by 0</t>
   </si>
 </sst>
 </file>
@@ -895,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2180,7 +2189,7 @@
         <v>139</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2399,7 +2408,7 @@
       <c r="L35" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N35" s="10" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2708,7 +2717,7 @@
         <v>139</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2928,7 +2937,7 @@
         <v>139</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2971,8 +2980,11 @@
       <c r="L48" s="8" t="s">
         <v>139</v>
       </c>
+      <c r="M48" t="s">
+        <v>142</v>
+      </c>
       <c r="N48" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3109,7 +3121,7 @@
         <v>139</v>
       </c>
       <c r="N51" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3153,7 +3165,7 @@
         <v>139</v>
       </c>
       <c r="N52" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3196,7 +3208,10 @@
       <c r="L53" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="N53" s="8" t="s">
+      <c r="M53" t="s">
+        <v>141</v>
+      </c>
+      <c r="N53" s="10" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>